<commit_message>
Centered text fields and buttons
</commit_message>
<xml_diff>
--- a/swl_reports.xlsx
+++ b/swl_reports.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,12 +494,6 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
           <t>18-10-2024</t>
@@ -510,12 +504,150 @@
           <t>10:38</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ON4CJK</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Jose</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>JO11ub</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>ON1DDR</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Andre</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>JO11ub</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>18-10-2024</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>10:46</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>14.250</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>SSB</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>via RTL-SDR</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ON4CJK</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>jose</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>JO11ub</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>ON1DDR</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Jose</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>JO11ds</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>18-10-2024</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>11:19</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>14.250</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>SSB</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Mary Islands</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>